<commit_message>
added .tsv and .xlsx in tidy form
</commit_message>
<xml_diff>
--- a/data/survey_data.xlsx
+++ b/data/survey_data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtababbasi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08571E6-39AC-874E-9161-74C2E1764181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="25120" windowHeight="14440" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="tidy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -140,6 +141,27 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Season </t>
+  </si>
+  <si>
+    <t>Plot Number</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Callibration Issue </t>
+  </si>
+  <si>
+    <t>OL</t>
   </si>
 </sst>
 </file>
@@ -149,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,11 +184,13 @@
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="28"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
@@ -177,16 +201,23 @@
       <b/>
       <sz val="24"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,12 +365,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +763,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,7 +807,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -800,7 +832,7 @@
   <dimension ref="C3:AB28"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -903,294 +935,294 @@
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1231,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1410,14 +1442,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.5" style="1"/>
     <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
@@ -2010,11 +2042,17 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="J28" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
+      <c r="M28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -2033,11 +2071,17 @@
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="J29" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
+      <c r="M29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
@@ -2054,11 +2098,17 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
+      <c r="J30" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
+      <c r="M30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
@@ -2077,11 +2127,17 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="J31" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -2100,11 +2156,17 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="J32" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
+      <c r="M32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -2286,4 +2348,1113 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54F94DC-7F8C-A948-AD91-D3EE4FBBCD48}">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2013</v>
+      </c>
+      <c r="B2" s="22">
+        <v>41471</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2013</v>
+      </c>
+      <c r="B3" s="22">
+        <v>41471</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>33</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4" s="22">
+        <v>41471</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="22">
+        <v>41471</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6" s="22">
+        <v>41473</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>2013</v>
+      </c>
+      <c r="B7" s="22">
+        <v>41473</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>48</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="22">
+        <v>41473</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>29</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2013</v>
+      </c>
+      <c r="B9" s="22">
+        <v>41473</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>37</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="22">
+        <v>41505</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>52</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2013</v>
+      </c>
+      <c r="B11" s="22">
+        <v>41564</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>33</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2013</v>
+      </c>
+      <c r="B12" s="22">
+        <v>41564</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="22">
+        <v>41618</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2013</v>
+      </c>
+      <c r="B14" s="22">
+        <v>41618</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>45</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15" s="22">
+        <v>41619</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>41</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16" s="22">
+        <v>41590</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>117</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>126</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2013</v>
+      </c>
+      <c r="B18" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>132</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2013</v>
+      </c>
+      <c r="B19" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>113</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>122</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>107</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22" s="22">
+        <v>41591</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>115</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23" s="22">
+        <v>41648</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>2014</v>
+      </c>
+      <c r="B24" s="22">
+        <v>41648</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>36</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25" s="22">
+        <v>41711</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>51</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="22">
+        <v>41711</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>44</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="22">
+        <v>41711</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>146</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>2014</v>
+      </c>
+      <c r="B28" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>44</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>45</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>157</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>218</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>52</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38" s="22">
+        <v>42074</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="B39" s="22">
+        <v>42102</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40" s="22">
+        <v>42130</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>2014</v>
+      </c>
+      <c r="B41" s="22">
+        <v>42142</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>182</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>2014</v>
+      </c>
+      <c r="B42" s="22">
+        <v>42164</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>29</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>2014</v>
+      </c>
+      <c r="B43" s="22">
+        <v>42193</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>115</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44" s="22">
+        <v>42193</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>190</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>2014</v>
+      </c>
+      <c r="B45" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>37</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>2014</v>
+      </c>
+      <c r="B46" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>2014</v>
+      </c>
+      <c r="B47" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>48</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>2014</v>
+      </c>
+      <c r="B48" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>52</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>2014</v>
+      </c>
+      <c r="B49" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>35</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ADD NA VALS TO XLS
</commit_message>
<xml_diff>
--- a/data/survey_data.xlsx
+++ b/data/survey_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtababbasi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaya\Desktop\tfcb-homework01\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08571E6-39AC-874E-9161-74C2E1764181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3271A3-8127-4D04-84A5-BE4BB5504B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="25120" windowHeight="14440" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
     <sheet name="tidy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -763,7 +763,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -807,7 +807,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -835,27 +835,27 @@
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1"/>
-    <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" customWidth="1"/>
-    <col min="16" max="16" width="52.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="26.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="16" max="16" width="52.85546875" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
-    <col min="26" max="26" width="17.5" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="1"/>
+    <col min="20" max="20" width="11.42578125" style="1"/>
+    <col min="21" max="21" width="19.85546875" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" customWidth="1"/>
+    <col min="29" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" ht="79" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" ht="78.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C3" s="11" t="s">
         <v>20</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -891,7 +891,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -908,7 +908,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C8" s="17">
         <v>41471</v>
       </c>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C9" s="17">
         <v>41471</v>
       </c>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C10" s="17">
         <v>41471</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C11" s="17">
         <v>41471</v>
       </c>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C12" s="17">
         <v>41473</v>
       </c>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C13" s="17">
         <v>41473</v>
       </c>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C14" s="17">
         <v>41473</v>
       </c>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C15" s="18">
         <v>41473</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1287,7 +1287,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1304,7 +1304,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1321,7 +1321,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1338,7 +1338,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1355,7 +1355,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1372,7 +1372,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1389,7 +1389,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1398,7 +1398,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1407,22 +1407,22 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G25" s="5"/>
       <c r="L25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G26" s="5"/>
       <c r="L26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G27" s="5"/>
       <c r="L27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G28" s="5"/>
       <c r="L28" s="5"/>
       <c r="Q28" s="5"/>
@@ -1446,25 +1446,25 @@
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="45.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" style="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
-    <col min="15" max="19" width="11.5" style="1"/>
+    <col min="3" max="3" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="22.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="22.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="1" customWidth="1"/>
+    <col min="15" max="19" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C8" s="6">
         <v>41648</v>
       </c>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C9" s="6">
         <v>41648</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C10" s="6">
         <v>41711</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C11" s="6">
         <v>41711</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C12" s="6">
         <v>41711</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1804,7 +1804,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1829,7 +1829,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1854,7 +1854,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1871,7 +1871,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1888,7 +1888,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1905,7 +1905,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1922,7 +1922,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:17" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1941,7 +1941,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1958,7 +1958,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1975,7 +1975,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1992,7 +1992,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -2009,7 +2009,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2057,7 +2057,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C29" s="6">
         <v>28498</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C30" s="6">
         <v>28498</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C31" s="6">
         <v>28498</v>
       </c>
@@ -2142,7 +2142,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C32" s="6">
         <v>28498</v>
       </c>
@@ -2171,7 +2171,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C33" s="6">
         <v>28498</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2211,7 +2211,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2228,7 +2228,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2245,7 +2245,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2260,7 +2260,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2277,7 +2277,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="L39" s="5"/>
@@ -2287,7 +2287,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="L40" s="5"/>
@@ -2297,7 +2297,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="L41" s="5"/>
@@ -2307,34 +2307,34 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="L42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="L43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G44" s="5"/>
       <c r="L44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G45" s="5"/>
       <c r="L45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G46" s="5"/>
       <c r="L46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.4">
       <c r="G47" s="5"/>
       <c r="L47" s="5"/>
       <c r="Q47" s="5"/>
@@ -2355,21 +2355,21 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>37</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -2408,11 +2408,14 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
       <c r="G2" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2013</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2013</v>
       </c>
@@ -2451,11 +2454,14 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
       <c r="G4" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -2471,11 +2477,14 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
       <c r="G5" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2013</v>
       </c>
@@ -2498,7 +2507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -2521,7 +2530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2013</v>
       </c>
@@ -2544,7 +2553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2013</v>
       </c>
@@ -2590,7 +2599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -2613,7 +2622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2013</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -2659,7 +2668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2013</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2013</v>
       </c>
@@ -2705,7 +2714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2013</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -2751,7 +2760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2013</v>
       </c>
@@ -2774,7 +2783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2013</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -2820,7 +2829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2013</v>
       </c>
@@ -2843,7 +2852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2013</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2014</v>
       </c>
@@ -2889,7 +2898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2014</v>
       </c>
@@ -2912,7 +2921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2014</v>
       </c>
@@ -2935,7 +2944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -2958,7 +2967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2014</v>
       </c>
@@ -2981,7 +2990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2014</v>
       </c>
@@ -2994,11 +3003,17 @@
       <c r="D28" t="s">
         <v>0</v>
       </c>
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
       <c r="G28" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2014</v>
       </c>
@@ -3021,7 +3036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2014</v>
       </c>
@@ -3044,7 +3059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2014</v>
       </c>
@@ -3067,7 +3082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -3080,11 +3095,17 @@
       <c r="D32" t="s">
         <v>6</v>
       </c>
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>0</v>
+      </c>
       <c r="G32" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2014</v>
       </c>
@@ -3107,7 +3128,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2014</v>
       </c>
@@ -3120,11 +3141,17 @@
       <c r="D34" t="s">
         <v>7</v>
       </c>
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
       <c r="G34" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2014</v>
       </c>
@@ -3147,7 +3174,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -3170,7 +3197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2014</v>
       </c>
@@ -3193,7 +3220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2014</v>
       </c>
@@ -3216,7 +3243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -3232,11 +3259,14 @@
       <c r="E39" t="s">
         <v>3</v>
       </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
       <c r="G39" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -3246,11 +3276,20 @@
       <c r="C40">
         <v>3</v>
       </c>
+      <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>0</v>
+      </c>
       <c r="G40" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -3273,7 +3312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2014</v>
       </c>
@@ -3296,7 +3335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2014</v>
       </c>
@@ -3319,7 +3358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2014</v>
       </c>
@@ -3342,7 +3381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2014</v>
       </c>
@@ -3365,7 +3404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2014</v>
       </c>
@@ -3381,11 +3420,14 @@
       <c r="E46" t="s">
         <v>1</v>
       </c>
+      <c r="F46" t="s">
+        <v>0</v>
+      </c>
       <c r="G46" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2014</v>
       </c>
@@ -3408,7 +3450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2014</v>
       </c>
@@ -3431,7 +3473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2014</v>
       </c>

</xml_diff>